<commit_message>
update label of "enhanced" to "restored" on supp figures
</commit_message>
<xml_diff>
--- a/dynamic_occupancy_model/model_outputs/appendix_s2.xlsx
+++ b/dynamic_occupancy_model/model_outputs/appendix_s2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jensj\Documents\R\urban_pollinator_occupancy_model\dynamic_occupancy_model\model_outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46A4AEF-C978-4134-842C-120E1137C292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313FF592-E1B0-4A22-BC5A-4DF2C2827883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3980" yWindow="1200" windowWidth="13640" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="appendix_s2" sheetId="1" r:id="rId1"/>
@@ -452,15 +452,6 @@
     <t>total number of site visit occassions on which each species was detected. The total number of site visits was 18 sites * 6 visits * 3 years = 324 possible detection events.</t>
   </si>
   <si>
-    <t>the species-specific effect of julian date on detection. A value of "0" would indicate that a species's phenological peak was on the average survey date (approximately June 15). Positive values indicate that the species phenology peaks after the mean survey date, whereas negative values indicate that the species phenology peaks before the mean survey date.</t>
-  </si>
-  <si>
-    <t>the species-specific effect of julian date squared on detection. A negative value would indicate that a species declines in detectability before or after the peak date. A positive value (was not estimated for any of our species) would indicate an inversion of detection, with species being more detectable on the outside shoulders of the season. Lower (more negative values) indicate that a species phenology attenuates rapidly around the peak detection date (i.e., that the species has very short flight season).</t>
-  </si>
-  <si>
-    <t>old-school classification of pollen specialization. These values were taken from: https://jarrodfowler.com/pollen_specialist.html. Species with blank cells have no information and could be either polyleges or understudied oligoleges.</t>
-  </si>
-  <si>
     <t>degree is the number of plant species that a pollinator interacts with, calculated using the bipartite package</t>
   </si>
   <si>
@@ -513,6 +504,15 @@
   </si>
   <si>
     <t>d supplemented genus, z-score scaled</t>
+  </si>
+  <si>
+    <t>the species-specific effect of julian date on detection (estimated by our model). A value of "0" would indicate that a species's phenological peak was on the average survey date (approximately June 15). Positive values indicate that the species phenology peaks after the mean survey date, whereas negative values indicate that the species phenology peaks before the mean survey date.</t>
+  </si>
+  <si>
+    <t>the species-specific effect of julian date squared on detection (estimated by our model). A negative value would indicate that a species declines in detectability before or after the peak date. A positive value (was not estimated for any of our species) would indicate an inversion of detection, with species being more detectable on the outside shoulders of the season. Lower (more negative values) indicate that a species phenology attenuates rapidly around the peak detection date (i.e., that the species has very short flight season).</t>
+  </si>
+  <si>
+    <t>binary classification of pollen specialization. These values were taken from: https://jarrodfowler.com/pollen_specialist.html. Species with blank cells have no information and could be either polyleges or understudied oligoleges.</t>
   </si>
 </sst>
 </file>
@@ -1379,7 +1379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -9159,8 +9159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19074CFA-4DAC-4F0F-960C-16019A161A00}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9206,7 +9206,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="116" x14ac:dyDescent="0.35">
@@ -9214,7 +9214,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="58" x14ac:dyDescent="0.35">
@@ -9222,7 +9222,7 @@
         <v>133</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -9230,7 +9230,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
@@ -9238,7 +9238,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
@@ -9246,7 +9246,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -9254,7 +9254,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -9262,7 +9262,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -9270,7 +9270,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
@@ -9278,7 +9278,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
@@ -9286,7 +9286,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -9294,7 +9294,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -9302,7 +9302,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -9310,7 +9310,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -9318,7 +9318,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
@@ -9326,7 +9326,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
@@ -9334,7 +9334,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
@@ -9342,7 +9342,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -9350,7 +9350,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -9358,7 +9358,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -9366,7 +9366,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -9375,12 +9375,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9528,15 +9525,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F1B489F-F96D-479E-ACC7-9CDEE92B8D60}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920E0497-396F-4742-AE2D-6C75EC39CA7D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6bb89d3d-6079-407f-b660-62d51b039648"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9560,17 +9568,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920E0497-396F-4742-AE2D-6C75EC39CA7D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F1B489F-F96D-479E-ACC7-9CDEE92B8D60}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6bb89d3d-6079-407f-b660-62d51b039648"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>